<commit_message>
Päivitä tuonti excel pohja talvihoitoreiteille
</commit_message>
<xml_diff>
--- a/dev-resources/excel/harja_talvihoitoreitit_pohja.xlsx
+++ b/dev-resources/excel/harja_talvihoitoreitit_pohja.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panu.pasanen/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panu.pasanen/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCD6B4B-A192-D949-B0E2-28E8BFBE1E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAB04E6-B11F-A948-9198-EE194D1E0712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21040" activeTab="1" xr2:uid="{8084DE53-A81F-1C43-943B-FDF8486ACF4F}"/>
+    <workbookView xWindow="48280" yWindow="7120" windowWidth="30240" windowHeight="18880" xr2:uid="{8084DE53-A81F-1C43-943B-FDF8486ACF4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Reittien nimet &amp; kalusto" sheetId="3" r:id="rId1"/>
     <sheet name="Reittien tiedot" sheetId="1" r:id="rId2"/>
-    <sheet name="Valinnat" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Valinnat" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>HARJA Talvihoitoreitit</t>
   </si>
@@ -109,28 +109,28 @@
     <t>Reitin nimi</t>
   </si>
   <si>
-    <t>Reitti 1</t>
-  </si>
-  <si>
-    <t>Reitti 2</t>
-  </si>
-  <si>
     <t>Reitin tulee sisältää kaikki siihen kuuluvat tiet (myös rampit, kiertoliittymät ja käpy-väylät). Ei hoitourakkaan kuulumattomia tietä, esim. katuja.</t>
   </si>
   <si>
     <t>Kaikki tiedot ovat pakollisia täyttää</t>
   </si>
   <si>
-    <t>Reitti 3</t>
-  </si>
-  <si>
-    <t>Pituus (km)*</t>
-  </si>
-  <si>
     <t>Reitti tunnistetaan nimen perusteella. Varmista, että kaikilla saman reitin tieosilla on sama nimi. Reitin nimet määritellään toisella välilehdellä.</t>
   </si>
   <si>
     <t>Täytä tälle välilehdelle reittien nimet sekä kalustomäärät</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Pituus (m)*</t>
   </si>
 </sst>
 </file>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D23A41-46FD-E04F-AF81-66B157584D36}">
   <dimension ref="A1:L550"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,7 +685,7 @@
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="F2" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -725,39 +725,21 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="11">
-        <v>1</v>
-      </c>
-      <c r="C5" s="11">
-        <v>2</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="11"/>
-      <c r="C6" s="11">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11">
-        <v>1</v>
-      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="11">
-        <v>2</v>
-      </c>
-      <c r="C7" s="11">
-        <v>1</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -3527,8 +3509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0389D453-6774-C346-BDCD-6729BBE93D77}">
   <dimension ref="A1:K499"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3547,18 +3529,18 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -3594,34 +3576,15 @@
         <v>9</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="11">
-        <v>1</v>
-      </c>
-      <c r="C6" s="11">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11">
-        <v>0</v>
-      </c>
-      <c r="E6" s="11">
-        <v>2</v>
-      </c>
-      <c r="F6" s="11">
-        <v>1000</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="20">
-        <v>10.5</v>
-      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
@@ -7081,17 +7044,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E6DEC995-95A5-504C-AA6E-6772657DF3BE}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B12BBDA6-711F-9947-BECE-6CBFE64FF1B5}">
           <x14:formula1>
-            <xm:f>Valinnat!$B$2:$B$7</xm:f>
+            <xm:f>Valinnat!$B$2:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>G6:G11</xm:sqref>
+          <xm:sqref>G6:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D083EA11-45FB-9341-8547-F2B9215176DF}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{678C7DB7-CB21-0F43-984F-23641463B6AF}">
           <x14:formula1>
-            <xm:f>'Reittien nimet &amp; kalusto'!$A$5:$A$151</xm:f>
+            <xm:f>'Reittien nimet &amp; kalusto'!$A$5:$A$1630</xm:f>
           </x14:formula1>
-          <xm:sqref>A6:A14 A15:A549</xm:sqref>
+          <xm:sqref>A6:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7101,10 +7064,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EBEDAB-8F2F-AB43-8B7B-BD67278C69D1}">
-  <dimension ref="B1:B7"/>
+  <dimension ref="B1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7147,6 +7110,21 @@
         <v>17</v>
       </c>
     </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>